<commit_message>
Add Datas of prison-copes & doctors in XML
</commit_message>
<xml_diff>
--- a/DATA/Role/charactor.xlsx
+++ b/DATA/Role/charactor.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="145">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -356,36 +356,6 @@
     <t>102</t>
   </si>
   <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
     <t>GEEK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -401,18 +371,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>normal</t>
-  </si>
-  <si>
     <t>Body_up</t>
   </si>
   <si>
-    <t>fat</t>
-  </si>
-  <si>
-    <t>thin</t>
-  </si>
-  <si>
     <t>RED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,10 +382,125 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>strong</t>
-  </si>
-  <si>
     <t>OLD FISH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>102_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g10_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g11_kidnap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIKMAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIC MICKEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHANE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR SLAVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BELLY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GORDON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOCTOR SNLAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAD DOCTOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COOK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>doctor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOCTOR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -529,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E113" tableType="xml" totalsRowShown="0" connectionId="2">
-  <autoFilter ref="A1:E113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E118" tableType="xml" totalsRowShown="0" connectionId="2">
+  <autoFilter ref="A1:E118"/>
   <tableColumns count="5">
     <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="4">
       <xmlColumnPr mapId="2" xpath="/Root/Charactor/@Name" xmlDataType="string"/>
@@ -839,15 +915,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" customWidth="1"/>
+    <col min="2" max="5" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -869,87 +946,77 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1828,104 +1895,218 @@
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="1"/>
       <c r="B104" s="1" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A105" s="1"/>
+      <c r="A105" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="B105" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C105" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
+      <c r="E105" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A106" s="1"/>
+      <c r="A106" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="B106" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C106" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
+      <c r="E106" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A107" s="1"/>
+      <c r="A107" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="B107" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C107" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
+      <c r="E107" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A108" s="1"/>
+      <c r="A108" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="B108" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="B109" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C109" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
+      <c r="E109" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="B110" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C110" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
+      <c r="E110" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="B111" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C111" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
+      <c r="E111" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A112" s="1"/>
+      <c r="A112" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="B112" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C112" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
+      <c r="E112" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A113" s="1"/>
+      <c r="A113" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="B113" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C113" s="1"/>
+        <v>125</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="E113" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A116" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A118" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>"Leg_up,Body_up"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>"normal,brown,grey,white"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D119:D1048576">
+      <formula1>"_b,_g,_w,,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
-      <formula1>"fat,thin,strong"</formula1>
+      <formula1>"1,2,3,g,doctor"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D118">
+      <formula1>"_b,_g,_w"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>